<commit_message>
Added updated BOM files and gerber
</commit_message>
<xml_diff>
--- a/KiCAD_project/CalculationGain.xlsx
+++ b/KiCAD_project/CalculationGain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/work/CUSTOM_ZDC_FIFO/KiCAD_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B6D69E-774E-144A-9F61-24775F892BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BFB04D-61CC-264F-86C4-978D94CE5BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37720" yWindow="560" windowWidth="28040" windowHeight="17120" xr2:uid="{3C194A3F-986B-144B-A3E5-2971A0502443}"/>
+    <workbookView xWindow="71400" yWindow="1200" windowWidth="28040" windowHeight="17120" xr2:uid="{3C194A3F-986B-144B-A3E5-2971A0502443}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>COEF</t>
   </si>
@@ -48,6 +48,21 @@
   </si>
   <si>
     <t>Rvar=</t>
+  </si>
+  <si>
+    <t>Vmax</t>
+  </si>
+  <si>
+    <t>Rfeedback</t>
+  </si>
+  <si>
+    <t>Rtrim</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>Trimmer is 1k</t>
   </si>
 </sst>
 </file>
@@ -430,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CEC43A6-3A82-2045-B43B-82C04A8B12BC}">
-  <dimension ref="B1:F205"/>
+  <dimension ref="B1:M205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,7 +456,7 @@
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -449,7 +464,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>0</v>
       </c>
@@ -458,7 +478,7 @@
         <v>1.2549999999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>1</v>
       </c>
@@ -472,8 +492,14 @@
       <c r="F6" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2</v>
       </c>
@@ -487,8 +513,14 @@
       <c r="F7">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>3</v>
       </c>
@@ -496,8 +528,14 @@
         <f t="shared" si="0"/>
         <v>1.2257281553398058</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>4</v>
       </c>
@@ -506,7 +544,7 @@
         <v>1.2163461538461537</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>5</v>
       </c>
@@ -514,8 +552,15 @@
         <f t="shared" si="0"/>
         <v>1.2071428571428573</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10">
+        <f>M6*M7/M8/2</f>
+        <v>0.61475409836065575</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>6</v>
       </c>
@@ -524,7 +569,7 @@
         <v>1.1981132075471699</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>7</v>
       </c>
@@ -533,7 +578,7 @@
         <v>1.1892523364485981</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>8</v>
       </c>
@@ -542,7 +587,7 @@
         <v>1.1805555555555556</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>9</v>
       </c>
@@ -551,7 +596,7 @@
         <v>1.1720183486238533</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>10</v>
       </c>
@@ -560,7 +605,7 @@
         <v>1.1636363636363636</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
v0.1 -> JLCPCB order
</commit_message>
<xml_diff>
--- a/KiCAD_project/CalculationGain.xlsx
+++ b/KiCAD_project/CalculationGain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/work/CUSTOM_ZDC_FIFO/KiCAD_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9A6735-82BF-4247-9724-6D6DE4428917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44F98F7-BE21-C048-9F3F-25DC2CAA59E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1560" windowWidth="28040" windowHeight="17120" xr2:uid="{3C194A3F-986B-144B-A3E5-2971A0502443}"/>
+    <workbookView xWindow="35260" yWindow="80" windowWidth="30240" windowHeight="17200" xr2:uid="{3C194A3F-986B-144B-A3E5-2971A0502443}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
   <dimension ref="B1:M205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2311,7 +2311,7 @@
         <v>200</v>
       </c>
       <c r="C205" s="3">
-        <f t="shared" si="3"/>
+        <f>(1+(390/($F$6+B205)))/4</f>
         <v>0.57499999999999996</v>
       </c>
     </row>

</xml_diff>